<commit_message>
Updated pinout for launchpad
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Pins.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Pins.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Launchpad" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
   <si>
     <t>PA2</t>
   </si>
@@ -24,9 +22,6 @@
     <t>Pin</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>PA3</t>
   </si>
   <si>
@@ -127,6 +122,195 @@
   </si>
   <si>
     <t>PF4</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>U1Rx</t>
+  </si>
+  <si>
+    <t>U1Tx</t>
+  </si>
+  <si>
+    <t>T2CCP0</t>
+  </si>
+  <si>
+    <t>T2CCP1</t>
+  </si>
+  <si>
+    <t>I2C1SCL</t>
+  </si>
+  <si>
+    <t>I2C1SDA</t>
+  </si>
+  <si>
+    <t>I2C0SCl</t>
+  </si>
+  <si>
+    <t>T3CCP0</t>
+  </si>
+  <si>
+    <t>I2C0SDA</t>
+  </si>
+  <si>
+    <t>T3CCP1</t>
+  </si>
+  <si>
+    <t>SSI2CLK</t>
+  </si>
+  <si>
+    <t>T1CCP0</t>
+  </si>
+  <si>
+    <t>CAN0RX</t>
+  </si>
+  <si>
+    <t>SSI0Tx</t>
+  </si>
+  <si>
+    <t>SSI0Rx</t>
+  </si>
+  <si>
+    <t>SSI0Fss</t>
+  </si>
+  <si>
+    <t>SSI0Clk</t>
+  </si>
+  <si>
+    <t>SSI2Tx</t>
+  </si>
+  <si>
+    <t>T0CCP1</t>
+  </si>
+  <si>
+    <t>T0CCP0</t>
+  </si>
+  <si>
+    <t>SSI2Rx</t>
+  </si>
+  <si>
+    <t>U4Rx</t>
+  </si>
+  <si>
+    <t>U5Rx</t>
+  </si>
+  <si>
+    <t>U4Tx</t>
+  </si>
+  <si>
+    <t>U3Rx</t>
+  </si>
+  <si>
+    <t>U3Tx</t>
+  </si>
+  <si>
+    <t>Wt0CCP0</t>
+  </si>
+  <si>
+    <t>Wt0CCP1</t>
+  </si>
+  <si>
+    <t>Wt1CCP0</t>
+  </si>
+  <si>
+    <t>Wt1CCP1</t>
+  </si>
+  <si>
+    <t>SSI3Clk</t>
+  </si>
+  <si>
+    <t>SSI3Fss</t>
+  </si>
+  <si>
+    <t>SSI3Rx</t>
+  </si>
+  <si>
+    <t>SSI3Tx</t>
+  </si>
+  <si>
+    <t>SSI1Clk</t>
+  </si>
+  <si>
+    <t>SSI1Fss</t>
+  </si>
+  <si>
+    <t>SSI1Rx</t>
+  </si>
+  <si>
+    <t>SSI1Tx</t>
+  </si>
+  <si>
+    <t>I2C3SCL</t>
+  </si>
+  <si>
+    <t>I2C3SDA</t>
+  </si>
+  <si>
+    <t>Wt2CCP0</t>
+  </si>
+  <si>
+    <t>Wt2CCP1</t>
+  </si>
+  <si>
+    <t>Wt3CCP0</t>
+  </si>
+  <si>
+    <t>Wt3CCP1</t>
+  </si>
+  <si>
+    <t>U2Rx</t>
+  </si>
+  <si>
+    <t>U2Tx</t>
+  </si>
+  <si>
+    <t>Wt5CCP0</t>
+  </si>
+  <si>
+    <t>Wt5CCP1</t>
+  </si>
+  <si>
+    <t>U7Rx</t>
+  </si>
+  <si>
+    <t>U1RTS</t>
+  </si>
+  <si>
+    <t>CAN0Rx</t>
+  </si>
+  <si>
+    <t>C0o</t>
+  </si>
+  <si>
+    <t>U7Tx</t>
+  </si>
+  <si>
+    <t>U5Tx</t>
+  </si>
+  <si>
+    <t>I2C2SCL</t>
+  </si>
+  <si>
+    <t>I2C2SDA</t>
+  </si>
+  <si>
+    <t>CAN0Tx</t>
+  </si>
+  <si>
+    <t>U1CTS</t>
+  </si>
+  <si>
+    <t>C1o</t>
+  </si>
+  <si>
+    <t>TRD1</t>
+  </si>
+  <si>
+    <t>SSI1Fs</t>
+  </si>
+  <si>
+    <t>T1CCP1</t>
   </si>
 </sst>
 </file>
@@ -150,12 +334,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,9 +360,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,200 +671,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J12" sqref="J12:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="J6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="J9" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" t="s">
+        <v>91</v>
+      </c>
+      <c r="N12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="J13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J15" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" t="s">
+        <v>95</v>
+      </c>
+      <c r="P15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="K16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="K17" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Ribbon cable and RS transceivers
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Pins.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Pins.xlsx
@@ -366,10 +366,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,26 +687,26 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -804,7 +804,7 @@
       <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>81</v>
       </c>
       <c r="M6" t="s">
@@ -821,7 +821,7 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>82</v>
       </c>
       <c r="M7" t="s">
@@ -832,7 +832,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E8" t="s">
@@ -841,7 +841,7 @@
       <c r="I8" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -849,7 +849,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E9" t="s">
@@ -858,7 +858,7 @@
       <c r="I9" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -906,7 +906,7 @@
       <c r="I12" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L12" t="s">
@@ -926,7 +926,7 @@
       <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="L13" t="s">
@@ -998,7 +998,7 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E16" t="s">
@@ -1018,7 +1018,7 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E17" t="s">
@@ -1041,7 +1041,7 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E18" t="s">
@@ -1058,7 +1058,7 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E19" t="s">

</xml_diff>